<commit_message>
Doan day code 16/4/2019 (fix loi)
</commit_message>
<xml_diff>
--- a/Document/4.Test/190408_Loi_DeXuatSua.xlsx
+++ b/Document/4.Test/190408_Loi_DeXuatSua.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2476AF-7D6F-4739-B20E-2A45A2B5C6CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB14A08-EDE9-4230-8719-E8195FD0A321}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>TT</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Click vào chi tiết 1 hàng hóa trong kho -&gt; Export ra file nhưng không mở được</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Ấn Ctr + F5 trên trình duyệt</t>
   </si>
 </sst>
 </file>
@@ -190,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +218,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -305,6 +317,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,7 +627,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -680,35 +713,37 @@
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="20">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="17">
         <v>43563</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="9"/>
+      <c r="J3" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
@@ -749,67 +784,67 @@
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="17">
         <v>43563</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="9"/>
+      <c r="J5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="19"/>
     </row>
     <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="17">
         <v>43391</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="9"/>
+      <c r="J6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
@@ -910,7 +945,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D1048576 D3:D5" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Lỗi, Đề xuất"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:J1048576 J3:J5" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"New, Resolve, Confirm, Close, Cancel, Accept"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>